<commit_message>
onderzoek data, wijzigingen david doorgevoerd
</commit_message>
<xml_diff>
--- a/Sprint 1/----_Database/Onderzoek-data.xlsx
+++ b/Sprint 1/----_Database/Onderzoek-data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jits\Documents\GitHub\vlambeerDocumenten\Sprint 1\----_Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -81,23 +86,23 @@
     <t>amount</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>House_Number</t>
-  </si>
-  <si>
-    <t>Postal</t>
+    <t>city</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>house_nr</t>
+  </si>
+  <si>
+    <t>postalcode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +113,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,12 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,7 +420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,7 +431,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,33 +443,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -496,75 +496,87 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
+      <c r="A12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
+      <c r="A14" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
onderzoek data, wijzigingen maarten doorgevoerd
</commit_message>
<xml_diff>
--- a/Sprint 1/----_Database/Onderzoek-data.xlsx
+++ b/Sprint 1/----_Database/Onderzoek-data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>user_id</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>postalcode</t>
+  </si>
+  <si>
+    <t>city2</t>
+  </si>
+  <si>
+    <t>street2</t>
+  </si>
+  <si>
+    <t>house_nr2</t>
+  </si>
+  <si>
+    <t>postalcode2</t>
   </si>
 </sst>
 </file>
@@ -430,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,75 +532,87 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
+      <c r="A15" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
+      <c r="A16" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
+      <c r="A17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
+      <c r="A18" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>